<commit_message>
updated Readme.MD also discovered issued fips-county crosswalk (st. names were off).
</commit_message>
<xml_diff>
--- a/national_county_edit.xlsx
+++ b/national_county_edit.xlsx
@@ -13351,8 +13351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3223"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A1291" workbookViewId="0">
+      <selection activeCell="F1310" sqref="F1310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15123,7 +15123,7 @@
         <v>4</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>2485</v>
+        <v>2486</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -15143,7 +15143,7 @@
         <v>4</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -16543,7 +16543,7 @@
         <v>4</v>
       </c>
       <c r="F159" s="4" t="s">
-        <v>2539</v>
+        <v>2540</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -16563,7 +16563,7 @@
         <v>4</v>
       </c>
       <c r="F160" s="4" t="s">
-        <v>2540</v>
+        <v>2541</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -16583,7 +16583,7 @@
         <v>4</v>
       </c>
       <c r="F161" s="4" t="s">
-        <v>2541</v>
+        <v>2542</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -16603,7 +16603,7 @@
         <v>4</v>
       </c>
       <c r="F162" s="4" t="s">
-        <v>2542</v>
+        <v>2543</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -16623,7 +16623,7 @@
         <v>4</v>
       </c>
       <c r="F163" s="4" t="s">
-        <v>2543</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -16643,7 +16643,7 @@
         <v>4</v>
       </c>
       <c r="F164" s="4" t="s">
-        <v>2544</v>
+        <v>2545</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -16663,7 +16663,7 @@
         <v>4</v>
       </c>
       <c r="F165" s="4" t="s">
-        <v>2545</v>
+        <v>2539</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -20883,7 +20883,7 @@
         <v>4</v>
       </c>
       <c r="F376" s="4" t="s">
-        <v>2729</v>
+        <v>2731</v>
       </c>
     </row>
     <row r="377" spans="1:6" x14ac:dyDescent="0.25">
@@ -20903,7 +20903,7 @@
         <v>4</v>
       </c>
       <c r="F377" s="4" t="s">
-        <v>2730</v>
+        <v>2732</v>
       </c>
     </row>
     <row r="378" spans="1:6" x14ac:dyDescent="0.25">
@@ -20923,7 +20923,7 @@
         <v>4</v>
       </c>
       <c r="F378" s="4" t="s">
-        <v>2731</v>
+        <v>2733</v>
       </c>
     </row>
     <row r="379" spans="1:6" x14ac:dyDescent="0.25">
@@ -20943,7 +20943,7 @@
         <v>4</v>
       </c>
       <c r="F379" s="4" t="s">
-        <v>2732</v>
+        <v>2729</v>
       </c>
     </row>
     <row r="380" spans="1:6" x14ac:dyDescent="0.25">
@@ -20963,7 +20963,7 @@
         <v>4</v>
       </c>
       <c r="F380" s="4" t="s">
-        <v>2733</v>
+        <v>2730</v>
       </c>
     </row>
     <row r="381" spans="1:6" x14ac:dyDescent="0.25">
@@ -28923,7 +28923,7 @@
         <v>4</v>
       </c>
       <c r="F778" s="4" t="s">
-        <v>2485</v>
+        <v>2540</v>
       </c>
     </row>
     <row r="779" spans="1:6" x14ac:dyDescent="0.25">
@@ -28943,7 +28943,7 @@
         <v>4</v>
       </c>
       <c r="F779" s="4" t="s">
-        <v>2540</v>
+        <v>2977</v>
       </c>
     </row>
     <row r="780" spans="1:6" x14ac:dyDescent="0.25">
@@ -28963,7 +28963,7 @@
         <v>4</v>
       </c>
       <c r="F780" s="4" t="s">
-        <v>2977</v>
+        <v>2978</v>
       </c>
     </row>
     <row r="781" spans="1:6" x14ac:dyDescent="0.25">
@@ -28983,7 +28983,7 @@
         <v>4</v>
       </c>
       <c r="F781" s="4" t="s">
-        <v>2978</v>
+        <v>2541</v>
       </c>
     </row>
     <row r="782" spans="1:6" x14ac:dyDescent="0.25">
@@ -29003,7 +29003,7 @@
         <v>4</v>
       </c>
       <c r="F782" s="4" t="s">
-        <v>2541</v>
+        <v>2486</v>
       </c>
     </row>
     <row r="783" spans="1:6" x14ac:dyDescent="0.25">
@@ -29023,7 +29023,7 @@
         <v>4</v>
       </c>
       <c r="F783" s="4" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
     </row>
     <row r="784" spans="1:6" x14ac:dyDescent="0.25">
@@ -37603,7 +37603,7 @@
         <v>4</v>
       </c>
       <c r="F1212" s="4" t="s">
-        <v>3220</v>
+        <v>3221</v>
       </c>
     </row>
     <row r="1213" spans="1:6" x14ac:dyDescent="0.25">
@@ -37623,7 +37623,7 @@
         <v>4</v>
       </c>
       <c r="F1213" s="4" t="s">
-        <v>3221</v>
+        <v>3220</v>
       </c>
     </row>
     <row r="1214" spans="1:6" x14ac:dyDescent="0.25">
@@ -41063,7 +41063,7 @@
         <v>4</v>
       </c>
       <c r="F1385" s="4" t="s">
-        <v>3342</v>
+        <v>2541</v>
       </c>
     </row>
     <row r="1386" spans="1:6" x14ac:dyDescent="0.25">
@@ -41083,7 +41083,7 @@
         <v>4</v>
       </c>
       <c r="F1386" s="4" t="s">
-        <v>2541</v>
+        <v>3343</v>
       </c>
     </row>
     <row r="1387" spans="1:6" x14ac:dyDescent="0.25">
@@ -41103,7 +41103,7 @@
         <v>4</v>
       </c>
       <c r="F1387" s="4" t="s">
-        <v>3343</v>
+        <v>3344</v>
       </c>
     </row>
     <row r="1388" spans="1:6" x14ac:dyDescent="0.25">
@@ -41123,7 +41123,7 @@
         <v>4</v>
       </c>
       <c r="F1388" s="4" t="s">
-        <v>3344</v>
+        <v>3342</v>
       </c>
     </row>
     <row r="1389" spans="1:6" x14ac:dyDescent="0.25">
@@ -53923,7 +53923,7 @@
         <v>4</v>
       </c>
       <c r="F2028" s="4" t="s">
-        <v>3672</v>
+        <v>3673</v>
       </c>
     </row>
     <row r="2029" spans="1:6" x14ac:dyDescent="0.25">
@@ -53943,7 +53943,7 @@
         <v>4</v>
       </c>
       <c r="F2029" s="4" t="s">
-        <v>3673</v>
+        <v>3674</v>
       </c>
     </row>
     <row r="2030" spans="1:6" x14ac:dyDescent="0.25">
@@ -53963,7 +53963,7 @@
         <v>4</v>
       </c>
       <c r="F2030" s="4" t="s">
-        <v>3674</v>
+        <v>3675</v>
       </c>
     </row>
     <row r="2031" spans="1:6" x14ac:dyDescent="0.25">
@@ -53983,7 +53983,7 @@
         <v>4</v>
       </c>
       <c r="F2031" s="4" t="s">
-        <v>3675</v>
+        <v>2978</v>
       </c>
     </row>
     <row r="2032" spans="1:6" x14ac:dyDescent="0.25">
@@ -54003,7 +54003,7 @@
         <v>4</v>
       </c>
       <c r="F2032" s="4" t="s">
-        <v>2978</v>
+        <v>3676</v>
       </c>
     </row>
     <row r="2033" spans="1:6" x14ac:dyDescent="0.25">
@@ -54023,7 +54023,7 @@
         <v>4</v>
       </c>
       <c r="F2033" s="4" t="s">
-        <v>3676</v>
+        <v>3672</v>
       </c>
     </row>
     <row r="2034" spans="1:6" x14ac:dyDescent="0.25">
@@ -75943,7 +75943,7 @@
         <v>4</v>
       </c>
       <c r="F3129" s="4" t="s">
-        <v>4287</v>
+        <v>4288</v>
       </c>
     </row>
     <row r="3130" spans="1:6" x14ac:dyDescent="0.25">
@@ -75963,7 +75963,7 @@
         <v>4</v>
       </c>
       <c r="F3130" s="4" t="s">
-        <v>4288</v>
+        <v>4289</v>
       </c>
     </row>
     <row r="3131" spans="1:6" x14ac:dyDescent="0.25">
@@ -75983,7 +75983,7 @@
         <v>4</v>
       </c>
       <c r="F3131" s="4" t="s">
-        <v>4289</v>
+        <v>4290</v>
       </c>
     </row>
     <row r="3132" spans="1:6" x14ac:dyDescent="0.25">
@@ -76003,7 +76003,7 @@
         <v>4</v>
       </c>
       <c r="F3132" s="4" t="s">
-        <v>4290</v>
+        <v>4291</v>
       </c>
     </row>
     <row r="3133" spans="1:6" x14ac:dyDescent="0.25">
@@ -76023,7 +76023,7 @@
         <v>4</v>
       </c>
       <c r="F3133" s="4" t="s">
-        <v>4291</v>
+        <v>4287</v>
       </c>
     </row>
     <row r="3134" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated readme with instructions
</commit_message>
<xml_diff>
--- a/national_county_edit.xlsx
+++ b/national_county_edit.xlsx
@@ -13351,8 +13351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1291" workbookViewId="0">
-      <selection activeCell="F1310" sqref="F1310"/>
+    <sheetView tabSelected="1" topLeftCell="A1140" workbookViewId="0">
+      <selection activeCell="F1160" sqref="F1160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50723,7 +50723,7 @@
         <v>4</v>
       </c>
       <c r="F1868" s="4" t="s">
-        <v>3058</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="1869" spans="1:6" x14ac:dyDescent="0.25">
@@ -50743,7 +50743,7 @@
         <v>4</v>
       </c>
       <c r="F1869" s="4" t="s">
-        <v>2472</v>
+        <v>3058</v>
       </c>
     </row>
     <row r="1870" spans="1:6" x14ac:dyDescent="0.25">
@@ -76743,7 +76743,7 @@
         <v>4</v>
       </c>
       <c r="F3169" s="4" t="s">
-        <v>3502</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="3170" spans="1:6" x14ac:dyDescent="0.25">
@@ -76763,7 +76763,7 @@
         <v>4</v>
       </c>
       <c r="F3170" s="4" t="s">
-        <v>2474</v>
+        <v>2475</v>
       </c>
     </row>
     <row r="3171" spans="1:6" x14ac:dyDescent="0.25">
@@ -76783,7 +76783,7 @@
         <v>4</v>
       </c>
       <c r="F3171" s="4" t="s">
-        <v>2475</v>
+        <v>2964</v>
       </c>
     </row>
     <row r="3172" spans="1:6" x14ac:dyDescent="0.25">
@@ -76803,7 +76803,7 @@
         <v>4</v>
       </c>
       <c r="F3172" s="4" t="s">
-        <v>2964</v>
+        <v>3502</v>
       </c>
     </row>
     <row r="3173" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>